<commit_message>
Alteração para usar multithreading
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Controle de temperatura" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,59 +422,85 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="39" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Dia do Mês</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Temperatura (C)</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Umidade</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Hora da Leitura</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Temperatura Média (C)</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Farmácia Rio Negro - Silva &amp; Heidrich ltda</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>31/12/2022</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Controle de temperatura - Sensor DHT-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Temperatura (ºC)</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Umidade (%)</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Hora da Leitura</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Temperatura Média (ºC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>04/01/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C6" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18:50:22</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>20:56:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>